<commit_message>
Use different cadd resource. Add float checks for the table data. Sleep after deleting.
</commit_message>
<xml_diff>
--- a/src/test/resources/annotator_test.xlsx
+++ b/src/test/resources/annotator_test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>name</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>AnnotatorTestSelenium</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -611,7 +614,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -645,16 +648,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>171570151</v>
+        <v>158796</v>
       </c>
       <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
         <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6">

</xml_diff>